<commit_message>
fix semantic model 00021-wc_lang.xlsx and add easy-to-read version
</commit_message>
<xml_diff>
--- a/tests/fixtures/verification/cases/semantic/00021/00021-wc_lang.xlsx
+++ b/tests/fixtures/verification/cases/semantic/00021/00021-wc_lang.xlsx
@@ -5,14 +5,14 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_dev_repos/wc_sim/tests/fixtures/verification/cases/semantic/00021/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_dev_repos/wc_sim/tests/fixtures/verification/cases/semantic/00004/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="36140" windowHeight="4960" tabRatio="500" activeTab="5"/>
-    <workbookView xWindow="20" yWindow="5480" windowWidth="36580" windowHeight="4780" tabRatio="500" firstSheet="3" activeTab="11"/>
-    <workbookView xWindow="20" yWindow="10260" windowWidth="25600" windowHeight="4980" tabRatio="500" firstSheet="6" activeTab="12"/>
-    <workbookView xWindow="0" yWindow="15260" windowWidth="25600" windowHeight="6340" tabRatio="500" firstSheet="7" activeTab="16"/>
+    <workbookView xWindow="-22160" yWindow="460" windowWidth="21900" windowHeight="4300" tabRatio="500" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="-22160" yWindow="4800" windowWidth="21900" windowHeight="5220" tabRatio="500" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="-22140" yWindow="10120" windowWidth="22020" windowHeight="4140" tabRatio="500" firstSheet="5" activeTab="12"/>
+    <workbookView xWindow="-22420" yWindow="14340" windowWidth="22260" windowHeight="7020" tabRatio="500" firstSheet="9" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -4231,7 +4231,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="215">
   <si>
     <t>!!!ObjTables ObjTablesVersion='0.0.8' Date='2019-12-05 16:22:38'</t>
   </si>
@@ -4782,6 +4782,9 @@
     <t>gram / liter</t>
   </si>
   <si>
+    <t>Two reactions using two species in one compartment</t>
+  </si>
+  <si>
     <t>These MWs balance the reactions</t>
   </si>
   <si>
@@ -4842,43 +4845,37 @@
     <t>molecule / mole</t>
   </si>
   <si>
-    <t>Two reactions with two species in one compartment with a non-unit volume.</t>
-  </si>
-  <si>
-    <t>test_case_00021_pop_mass_independent</t>
+    <t>test_case_00004_pop_mass_independent</t>
   </si>
   <si>
     <t>abstract_compartment</t>
   </si>
   <si>
+    <t>Must equal volume of c in Compartments</t>
+  </si>
+  <si>
+    <t>1 / molecule</t>
+  </si>
+  <si>
+    <t>Units conversion</t>
+  </si>
+  <si>
+    <t>rl_units_conv</t>
+  </si>
+  <si>
+    <t>Avogadro * rl_units_conv</t>
+  </si>
+  <si>
     <t>conv</t>
   </si>
   <si>
+    <t>k1 * S1[c] * pop_2_conc * vol_c * conv</t>
+  </si>
+  <si>
+    <t>k2 * S2[c] * S2[c] * pop_2_conc**2 * vol_c * conv</t>
+  </si>
+  <si>
     <t>Conversion factor for rate laws</t>
-  </si>
-  <si>
-    <t>Avogadro * rl_units_conv</t>
-  </si>
-  <si>
-    <t>Must equal volume of c in Compartments</t>
-  </si>
-  <si>
-    <t>rl_units_conv</t>
-  </si>
-  <si>
-    <t>Units conversion</t>
-  </si>
-  <si>
-    <t>1 / molecule</t>
-  </si>
-  <si>
-    <t>k1 * S1[c] * pop_2_conc * vol_c * conv</t>
-  </si>
-  <si>
-    <t>k2 * S2[c] * S2[c] * pop_2_conc**2 * vol_c * conv</t>
-  </si>
-  <si>
-    <t>specified abundance is 1.4E-4 moles, which must be scaled volume != 1 liter</t>
   </si>
 </sst>
 </file>
@@ -4889,7 +4886,7 @@
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
     <numFmt numFmtId="165" formatCode="0.0000E+00"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4956,8 +4953,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4987,8 +4990,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -5005,13 +5014,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="5" tint="0.39994506668294322"/>
+      </left>
+      <right style="thin">
+        <color theme="5" tint="0.39994506668294322"/>
+      </right>
+      <top style="thin">
+        <color theme="5" tint="0.39994506668294322"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -5035,10 +5059,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -5102,38 +5148,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -5141,6 +5161,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -5741,14 +5764,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F4"/>
     </sheetView>
-    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1"/>
-    <sheetView showRowColHeaders="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="2"/>
-    <sheetView workbookViewId="3">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
+    <sheetView workbookViewId="3"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5939,21 +5960,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F4"/>
     </sheetView>
-    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1"/>
-    <sheetView showRowColHeaders="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="2"/>
-    <sheetView showRowColHeaders="0" workbookViewId="3">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="A3" sqref="A3:D4"/>
     </sheetView>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="2"/>
+    <sheetView workbookViewId="3"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="27.1640625" style="24" customWidth="1"/>
-    <col min="3" max="3" width="32.5" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.83203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.1640625" style="32" customWidth="1"/>
+    <col min="3" max="3" width="32.5" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" style="28" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="15.6640625" customWidth="1"/>
     <col min="8" max="8" width="38" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" customWidth="1"/>
@@ -5964,9 +5985,9 @@
       <c r="A1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -5977,13 +5998,13 @@
       <c r="A2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="26" t="s">
         <v>66</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -6004,16 +6025,16 @@
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>196</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>194</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>200</v>
+      <c r="D3" s="27" t="s">
+        <v>201</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -6023,16 +6044,16 @@
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>208</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>201</v>
+        <v>211</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>202</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -6042,9 +6063,9 @@
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -6053,9 +6074,9 @@
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -6064,9 +6085,9 @@
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -6075,59 +6096,39 @@
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <autoFilter ref="A2:I2"/>
   <dataValidations count="9">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="A9:A10">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="A7:A8">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B9:B10">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B7:B8">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." sqref="C9:C10"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Enter a unit or blank." sqref="D9:D10"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="E9:E10"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="F9:F10"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="G9:G10"/>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="H9:H10">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." sqref="C7:C8"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Enter a unit or blank." sqref="D7:D8"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="E7:E8"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="F7:F8"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="G7:G8"/>
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="H7:H8">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="I9:I10"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="I7:I8"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6138,14 +6139,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
-    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1"/>
-    <sheetView showRowColHeaders="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="2"/>
-    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="3">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="2"/>
+    <sheetView workbookViewId="3"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6178,13 +6177,13 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="47" t="s">
+      <c r="G2" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="I2" s="48" t="s">
+      <c r="I2" s="47" t="s">
         <v>86</v>
       </c>
       <c r="J2" s="5"/>
@@ -6209,7 +6208,7 @@
       <c r="E3" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="45" t="s">
         <v>90</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -6238,22 +6237,22 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="15" t="s">
         <v>170</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>184</v>
+      <c r="D4" s="15" t="s">
+        <v>185</v>
       </c>
       <c r="E4" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="42" t="s">
         <v>171</v>
       </c>
       <c r="G4" s="3"/>
@@ -6266,17 +6265,17 @@
       <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="15" t="s">
         <v>186</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>187</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>187</v>
+      <c r="D5" s="15" t="s">
+        <v>188</v>
       </c>
       <c r="E5" s="3" t="b">
         <v>0</v>
@@ -6458,7 +6457,7 @@
       <formula1>4294967295</formula1>
     </dataValidation>
     <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="N4:N13"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;1 / second&quot; or blank." sqref="F4:F5">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;1 / second&quot; or blank." sqref="F5">
       <formula1>"1 / second"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6483,16 +6482,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
-    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1"/>
-    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="2">
-      <selection activeCell="F3" sqref="F3:F4"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
-    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="3">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="2">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
+    <sheetView workbookViewId="3"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6564,19 +6563,19 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="19" t="s">
         <v>172</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="G3" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="G3" s="20" t="s">
         <v>180</v>
       </c>
       <c r="H3" s="3"/>
@@ -6586,20 +6585,20 @@
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>188</v>
+      <c r="A4" s="15" t="s">
+        <v>189</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="D4" s="11" t="s">
+      <c r="C4" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="D4" s="19" t="s">
         <v>172</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="G4" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="G4" s="20" t="s">
         <v>180</v>
       </c>
       <c r="H4" s="3"/>
@@ -6766,12 +6765,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
-    <sheetView showRowColHeaders="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
-    <sheetView showRowColHeaders="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="2"/>
-    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="3">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="2"/>
+    <sheetView workbookViewId="3"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7021,12 +7018,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView showRowColHeaders="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
-    <sheetView showRowColHeaders="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="2"/>
-    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="3">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
+    <sheetView workbookViewId="3"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7245,12 +7240,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView showRowColHeaders="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
-    <sheetView showRowColHeaders="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="2"/>
-    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="3">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
+    <sheetView workbookViewId="3"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7489,21 +7482,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView showRowColHeaders="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
-    <sheetView showRowColHeaders="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="2"/>
-    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="3">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="3">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="2" max="2" width="28.33203125" customWidth="1"/>
     <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="13" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="13" customWidth="1"/>
-    <col min="6" max="6" width="26.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="21" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="21" customWidth="1"/>
+    <col min="6" max="6" width="26.33203125" style="28" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="3" customWidth="1"/>
     <col min="9" max="9" width="2.6640625" customWidth="1"/>
     <col min="10" max="10" width="38" bestFit="1" customWidth="1"/>
@@ -7517,9 +7512,9 @@
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="17"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="25"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -7536,13 +7531,13 @@
       <c r="C2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="26" t="s">
         <v>66</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -7562,18 +7557,18 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="31">
+      <c r="B3" s="39"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="39">
         <v>0.35</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="36">
         <v>0</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="40" t="s">
         <v>171</v>
       </c>
       <c r="G3" s="3"/>
@@ -7583,19 +7578,19 @@
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
-        <v>189</v>
-      </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="31">
+      <c r="A4" s="39" t="s">
+        <v>190</v>
+      </c>
+      <c r="B4" s="39"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="39">
         <v>180</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="36">
         <v>0</v>
       </c>
-      <c r="F4" s="32" t="s">
-        <v>199</v>
+      <c r="F4" s="40" t="s">
+        <v>200</v>
       </c>
       <c r="K4" s="3"/>
     </row>
@@ -7604,16 +7599,16 @@
         <v>162</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="15">
+      <c r="D5" s="23">
         <v>1</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="23">
         <v>0</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="27" t="s">
         <v>182</v>
       </c>
       <c r="G5" s="3"/>
@@ -7623,72 +7618,73 @@
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="27" t="s">
-        <v>191</v>
-      </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="29">
+      <c r="A6" s="35" t="s">
+        <v>192</v>
+      </c>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="37">
         <v>6.0221408570000002E+23</v>
       </c>
-      <c r="E6" s="27"/>
-      <c r="F6" s="30" t="s">
-        <v>202</v>
-      </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="16" t="s">
-        <v>197</v>
+      <c r="E6" s="35"/>
+      <c r="F6" s="38" t="s">
+        <v>203</v>
+      </c>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="24" t="s">
+        <v>198</v>
       </c>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="45">
+        <v>194</v>
+      </c>
+      <c r="C7" s="27"/>
+      <c r="D7" s="43">
         <v>0.3</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="23">
         <v>0</v>
       </c>
-      <c r="F7" s="19" t="s">
-        <v>190</v>
+      <c r="F7" s="27" t="s">
+        <v>191</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="21" t="s">
-        <v>209</v>
+      <c r="J7" s="29" t="s">
+        <v>206</v>
       </c>
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="46">
+      <c r="D8" s="44">
         <v>1</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="23">
         <v>0</v>
       </c>
-      <c r="F8" s="19" t="s">
-        <v>212</v>
+      <c r="F8" s="27" t="s">
+        <v>207</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7696,33 +7692,6 @@
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <autoFilter ref="A2:K2"/>
-  <dataValidations count="11">
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="G6:G7"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="H6:H7"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="I6:I7"/>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="J6:J7">
-      <formula1>4294967295</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard error" error="Value must be a float or blank." promptTitle="Standard error" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="E6:E7">
-      <formula1>-1E-100</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="A6:A7">
-      <formula1>1</formula1>
-      <formula2>63</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value" error="Value must be a float or blank." promptTitle="Value" prompt="Enter a float or blank." sqref="D6:D7">
-      <formula1>-1E+100</formula1>
-      <formula2>1E+100</formula2>
-    </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="K6:K7"/>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B6:B7">
-      <formula1>255</formula1>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." sqref="C6:C7">
-      <formula1>"kinetic_constant,K_i,K_m,k_cat,v_max"</formula1>
-    </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Enter a unit or blank." sqref="F6:F7"/>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
@@ -7733,7 +7702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
     <sheetView workbookViewId="2"/>
     <sheetView workbookViewId="3"/>
@@ -7927,7 +7896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
     <sheetView workbookViewId="2"/>
     <sheetView workbookViewId="3"/>
@@ -7972,42 +7941,42 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="47" t="s">
+      <c r="G2" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="I2" s="47" t="s">
+      <c r="I2" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="J2" s="48" t="s">
+      <c r="J2" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="K2" s="48" t="s">
+      <c r="K2" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="L2" s="48" t="s">
+      <c r="L2" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="M2" s="48" t="s">
+      <c r="M2" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="N2" s="48" t="s">
+      <c r="N2" s="47" t="s">
         <v>108</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="47" t="s">
+      <c r="Q2" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="R2" s="48" t="s">
+      <c r="R2" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="S2" s="47" t="s">
+      <c r="S2" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="T2" s="48" t="s">
+      <c r="T2" s="47" t="s">
         <v>110</v>
       </c>
       <c r="U2" s="5"/>
@@ -8420,17 +8389,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
     <sheetView workbookViewId="2"/>
     <sheetView workbookViewId="3"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="60" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="12" width="8.83203125" customWidth="1"/>
     <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
   </cols>
@@ -8474,7 +8443,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -8885,10 +8854,10 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="47" t="s">
+      <c r="G2" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="47" t="s">
         <v>121</v>
       </c>
       <c r="I2" s="5"/>
@@ -10104,10 +10073,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
     <sheetView workbookViewId="2"/>
     <sheetView workbookViewId="3"/>
   </sheetViews>
@@ -10254,10 +10223,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F4"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
     <sheetView workbookViewId="2"/>
     <sheetView workbookViewId="3"/>
   </sheetViews>
@@ -10416,10 +10385,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F4"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
     <sheetView workbookViewId="2"/>
     <sheetView workbookViewId="3"/>
   </sheetViews>
@@ -10601,10 +10570,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
-    <sheetView showRowColHeaders="0" workbookViewId="1"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
     <sheetView workbookViewId="2"/>
     <sheetView workbookViewId="3"/>
   </sheetViews>
@@ -10647,29 +10616,29 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="47" t="s">
+      <c r="H2" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="48" t="s">
+      <c r="I2" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="48" t="s">
+      <c r="J2" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="48" t="s">
+      <c r="K2" s="47" t="s">
         <v>56</v>
       </c>
       <c r="L2" s="5"/>
-      <c r="M2" s="47" t="s">
+      <c r="M2" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="N2" s="48" t="s">
+      <c r="N2" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="O2" s="48" t="s">
+      <c r="O2" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="P2" s="48" t="s">
+      <c r="P2" s="47" t="s">
         <v>57</v>
       </c>
       <c r="Q2" s="5"/>
@@ -10694,7 +10663,7 @@
       <c r="E3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="41" t="s">
         <v>61</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -10743,68 +10712,68 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="34" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" t="s">
         <v>159</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36" t="s">
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="H4" s="37" t="s">
+      <c r="H4" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="I4" s="38">
-        <v>0.3</v>
-      </c>
-      <c r="J4" s="36">
+      <c r="I4" s="9">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3">
         <v>0</v>
       </c>
-      <c r="K4" s="39" t="s">
-        <v>190</v>
-      </c>
-      <c r="L4" s="37" t="s">
+      <c r="K4" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="L4" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="M4" s="36"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="36"/>
-      <c r="R4" s="36"/>
-      <c r="S4" s="36"/>
-      <c r="T4" s="36"/>
-      <c r="U4" s="36"/>
-    </row>
-    <row r="5" spans="1:21" s="34" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="37"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="36"/>
-      <c r="P5" s="36"/>
-      <c r="Q5" s="36"/>
-      <c r="R5" s="36"/>
-      <c r="S5" s="36"/>
-      <c r="T5" s="36"/>
-      <c r="U5" s="36"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+    </row>
+    <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="11"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
     </row>
     <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
@@ -10997,50 +10966,50 @@
     <mergeCell ref="M2:P2"/>
   </mergeCells>
   <dataValidations count="18">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="A9:A13">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="A4:A13">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B9:B13">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B4:B13">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Biological type" error="Value must be a comma-separated list of WC ontology terms &quot;cellular_compartment&quot;, &quot;extracellular_compartment&quot; or blank." promptTitle="Biological type" prompt="Enter a comma-separated list of WC ontology terms &quot;cellular_compartment&quot;, &quot;extracellular_compartment&quot; or blank." sqref="C9:C13">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Biological type" error="Value must be a comma-separated list of WC ontology terms &quot;cellular_compartment&quot;, &quot;extracellular_compartment&quot; or blank." promptTitle="Biological type" prompt="Enter a comma-separated list of WC ontology terms &quot;cellular_compartment&quot;, &quot;extracellular_compartment&quot; or blank." sqref="C4:C13">
       <formula1>"cellular_compartment,extracellular_compartment"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Physical type" error="Value must be a comma-separated list of WC ontology terms &quot;fluid_compartment&quot;, &quot;membrane_compartment&quot; or blank." promptTitle="Physical type" prompt="Enter a comma-separated list of WC ontology terms &quot;fluid_compartment&quot;, &quot;membrane_compartment&quot; or blank." sqref="D9:D13">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Physical type" error="Value must be a comma-separated list of WC ontology terms &quot;fluid_compartment&quot;, &quot;membrane_compartment&quot; or blank." promptTitle="Physical type" prompt="Enter a comma-separated list of WC ontology terms &quot;fluid_compartment&quot;, &quot;membrane_compartment&quot; or blank." sqref="D4:D13">
       <formula1>"fluid_compartment,membrane_compartment"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Geometry" error="Value must be a comma-separated list of WC ontology terms &quot;3D_compartment&quot; or blank." promptTitle="Geometry" prompt="Enter a comma-separated list of WC ontology terms &quot;3D_compartment&quot; or blank." sqref="E9:E13">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Geometry" error="Value must be a comma-separated list of WC ontology terms &quot;3D_compartment&quot; or blank." promptTitle="Geometry" prompt="Enter a comma-separated list of WC ontology terms &quot;3D_compartment&quot; or blank." sqref="E4:E13">
       <formula1>"3D_compartment"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Mass units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;gram&quot; or blank." promptTitle="Mass units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;gram&quot; or blank." sqref="G9:G13">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Mass units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;gram&quot; or blank." promptTitle="Mass units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;gram&quot; or blank." sqref="G4:G13">
       <formula1>"gram"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Mean" error="Value must be a float or blank." promptTitle="Mean" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="I9:I13">
+    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Mean" error="Value must be a float or blank." promptTitle="Mean" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="I4:I13">
       <formula1>-1E-100</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard deviation" error="Value must be a float or blank." promptTitle="Standard deviation" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="O9:O13 J9:J13">
+    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard deviation" error="Value must be a float or blank." promptTitle="Standard deviation" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="J4:J13 O4:O13">
       <formula1>-1E-100</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Distribution" error="Value must be a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;W ..." promptTitle="Distribution" prompt="Enter a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;Weibull_d ..." sqref="H9:H13 M9:M13"/>
-    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Mean" error="Value must be a float or blank." promptTitle="Mean" prompt="Enter a float or blank." sqref="N9:N13">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Distribution" error="Value must be a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;W ..." promptTitle="Distribution" prompt="Enter a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;Weibull_d ..." sqref="M4:M13 H4 H6:H13"/>
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Mean" error="Value must be a float or blank." promptTitle="Mean" prompt="Enter a float or blank." sqref="N4:N13">
       <formula1>-1E+100</formula1>
       <formula2>1E+100</formula2>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;dimensionless&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;dimensionless&quot; or blank." sqref="P9:P13">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;dimensionless&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;dimensionless&quot; or blank." sqref="P4:P13">
       <formula1>"dimensionless"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="Q9:Q13"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="R9:R13"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="S9:S13"/>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="T9:T13">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="Q4:Q13"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="R4:R13"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="S4:S13"/>
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="T4:T13">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="U9:U13"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;liter&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;liter&quot; or blank." sqref="K9:K13">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="U4:U13"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;liter&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;liter&quot; or blank." sqref="K6:K13 K4">
       <formula1>"liter"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Parent compartment" error="Value must be a value from &quot;!!Compartments:A&quot; or blank." promptTitle="Parent compartment" prompt="Select a value from &quot;!!Compartments:A&quot; or blank." sqref="F9:F13">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Parent compartment" error="Value must be a value from &quot;!!Compartments:A&quot; or blank." promptTitle="Parent compartment" prompt="Select a value from &quot;!!Compartments:A&quot; or blank." sqref="F4:F13">
       <formula1>$A$4:$A$1048576</formula1>
     </dataValidation>
   </dataValidations>
@@ -11048,12 +11017,18 @@
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Initial density" error="Value must be a value from &quot;!!Parameters:A&quot; or blank." promptTitle="Initial density" prompt="Select a value from &quot;!!Parameters:A&quot; or blank.">
           <x14:formula1>
             <xm:f>'!!Parameters'!$A$3:$A$1048576</xm:f>
           </x14:formula1>
-          <xm:sqref>L9:L13</xm:sqref>
+          <xm:sqref>L6:L13</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Initial density" error="Value must be a value from &quot;!!Parameters:A&quot; or blank." promptTitle="Initial density" prompt="Select a value from &quot;!!Parameters:A&quot; or blank.">
+          <x14:formula1>
+            <xm:f>'!!Parameters'!$A$3:$A$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>L4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -11065,11 +11040,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
-    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1"/>
-    <sheetView showRowColHeaders="0" workbookViewId="2"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
     <sheetView workbookViewId="3"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -11101,22 +11076,22 @@
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="E2" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="48" t="s">
+      <c r="F2" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="G2" s="48" t="s">
+      <c r="G2" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="47" t="s">
         <v>69</v>
       </c>
       <c r="I2" s="5"/>
@@ -11142,7 +11117,7 @@
       <c r="E3" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="41" t="s">
         <v>73</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -11187,14 +11162,14 @@
       <c r="H4" s="8">
         <v>0</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="14" t="s">
         <v>165</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="9" t="s">
-        <v>183</v>
+      <c r="M4" s="14" t="s">
+        <v>184</v>
       </c>
       <c r="N4" s="3"/>
     </row>
@@ -11215,14 +11190,14 @@
       <c r="H5" s="8">
         <v>0</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="14" t="s">
         <v>165</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
-      <c r="M5" s="9" t="s">
-        <v>183</v>
+      <c r="M5" s="14" t="s">
+        <v>184</v>
       </c>
       <c r="N5" s="3"/>
     </row>
@@ -11402,11 +11377,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F4"/>
     </sheetView>
-    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1"/>
-    <sheetView showRowColHeaders="0" workbookViewId="2"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
     <sheetView workbookViewId="3"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -11462,7 +11437,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="15" t="s">
         <v>166</v>
       </c>
       <c r="B3" s="3"/>
@@ -11482,7 +11457,7 @@
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="15" t="s">
         <v>167</v>
       </c>
       <c r="B4" s="3"/>
@@ -11644,19 +11619,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
-    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
-    <sheetView showRowColHeaders="0" workbookViewId="2"/>
+    <sheetView workbookViewId="2"/>
     <sheetView workbookViewId="3"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="12" width="15.6640625" customWidth="1"/>
+    <col min="1" max="12" width="15.6640625" customWidth="1"/>
     <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11714,73 +11688,71 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="34" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="41" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" t="s">
         <v>161</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="18">
         <v>1.4999999999999999E-4</v>
       </c>
-      <c r="F3" s="43">
+      <c r="F3" s="16">
         <v>0</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="G3" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36" t="s">
-        <v>215</v>
-      </c>
-      <c r="L3" s="36"/>
-    </row>
-    <row r="4" spans="1:12" s="34" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="36" t="s">
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="41" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" t="s">
         <v>161</v>
       </c>
-      <c r="E4" s="41">
+      <c r="E4" s="15">
         <v>0</v>
       </c>
-      <c r="F4" s="43">
+      <c r="F4" s="16">
         <v>0</v>
       </c>
-      <c r="G4" s="44" t="s">
+      <c r="G4" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-    </row>
-    <row r="5" spans="1:12" s="34" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
@@ -11883,29 +11855,29 @@
   </sheetData>
   <autoFilter ref="A2:L2"/>
   <dataValidations count="11">
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." promptTitle="Id" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." sqref="A9:A12">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." promptTitle="Id" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." sqref="A3:A12 C3:C4">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B9:B12">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B3:B12">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Distribution" error="Value must be a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;W ..." promptTitle="Distribution" prompt="Enter a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;Weibull_d ..." sqref="D9:D12"/>
-    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Mean" error="Value must be a float or blank." promptTitle="Mean" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="E9:E12">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Distribution" error="Value must be a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;W ..." promptTitle="Distribution" prompt="Enter a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;Weibull_d ..." sqref="D3:D12"/>
+    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Mean" error="Value must be a float or blank." promptTitle="Mean" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="E3:E12">
       <formula1>-1E-100</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard deviation" error="Value must be a float or blank." promptTitle="Standard deviation" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="F9:F12">
+    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard deviation" error="Value must be a float or blank." promptTitle="Standard deviation" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="F3:F12">
       <formula1>-1E-100</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." sqref="G9:G12">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." sqref="G3:G12">
       <formula1>"molecule,molar,millimolar,micromolar,nanomolar,picomolar,femtomolar,attomolar"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H9:H12"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="I9:I12"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J9:J12"/>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="K9:K12">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H3:H12"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="I3:I12"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J3:J12"/>
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="K3:K12">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L9:L12"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L3:L12"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -11916,7 +11888,7 @@
           <x14:formula1>
             <xm:f>'!!Species'!$A$3:$A$1048576</xm:f>
           </x14:formula1>
-          <xm:sqref>C9:C12</xm:sqref>
+          <xm:sqref>C5:C12</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>